<commit_message>
set up preliminary ML-kNN model
</commit_message>
<xml_diff>
--- a/dataset/content_paragraphs_v1.xlsx
+++ b/dataset/content_paragraphs_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/li_7232_buckeyemail_osu_edu/Documents/NewsArticleClassification/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/architdatar/repo/StatMachLearn/NewsArticleClassification/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{871D6A31-ACDF-4141-9FC8-C50CDE95712F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F856D255-705A-42B1-8DA3-EEBE192696E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE37ED3-C4E3-0643-B962-1E374FC35549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1381,23 +1381,23 @@
   <dimension ref="A1:X289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C293" sqref="C293"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.6328125" style="2" customWidth="1"/>
-    <col min="3" max="12" width="14.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" style="1" customWidth="1"/>
-    <col min="16" max="18" width="14.81640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.81640625" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86" style="2" customWidth="1"/>
+    <col min="3" max="12" width="14.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" style="1" customWidth="1"/>
+    <col min="16" max="18" width="14.83203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>214236</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>214232</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>214266</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>214246</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>214238</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>214249</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>214435</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>214253</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>214243</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>214244</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>214263</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>214245</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>214262</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>214265</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>214234</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>214231</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>214353</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>214437</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>214252</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>214271</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>214348</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>214361</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>214429</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>214261</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>214270</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>214358</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>214247</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>214427</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>214408</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>214298</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>214425</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>214237</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>214346</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>214430</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>214399</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>214365</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>214369</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>214422</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>214240</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>214251</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>214291</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>214313</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>214436</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>214439</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>214354</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>214286</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>214405</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>214432</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>214280</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>214351</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>214398</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>214424</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>214428</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>214397</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>214441</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>214340</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>214378</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>214264</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>214423</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>214248</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>214433</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>214198</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>214225</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>214273</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>214277</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>214296</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>214302</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>214360</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>214235</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>214326</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>214349</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>214387</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>214333</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>214334</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>214230</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>214267</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>214281</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>214228</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>214352</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>214342</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>214250</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>214282</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>214324</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>214269</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>214272</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>214293</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>214321</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>214350</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>214379</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>214386</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>214402</v>
       </c>
@@ -8205,7 +8205,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>214276</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>214292</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>214297</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>214345</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>214377</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>214401</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>214404</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>214406</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>214283</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>214370</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>214419</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>214355</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>214396</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>214421</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>214220</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>214221</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>214295</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>214290</v>
       </c>
@@ -9537,7 +9537,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>214227</v>
       </c>
@@ -9611,7 +9611,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>214256</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>214362</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>214415</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>214229</v>
       </c>
@@ -9907,7 +9907,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>214260</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>214278</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>214300</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>214317</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>214320</v>
       </c>
@@ -10277,7 +10277,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>214444</v>
       </c>
@@ -10351,7 +10351,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>214319</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>214384</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>214414</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>214274</v>
       </c>
@@ -10647,7 +10647,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>214312</v>
       </c>
@@ -10721,7 +10721,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>214388</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>214409</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>214303</v>
       </c>
@@ -10943,7 +10943,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>214310</v>
       </c>
@@ -11017,7 +11017,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>214323</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>214331</v>
       </c>
@@ -11165,7 +11165,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>214420</v>
       </c>
@@ -11239,7 +11239,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>214226</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>214279</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>214299</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>214301</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>214305</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>214308</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>214363</v>
       </c>
@@ -11757,7 +11757,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>214440</v>
       </c>
@@ -11831,7 +11831,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>214344</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>214359</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>214371</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>214383</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>214400</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>214339</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>214417</v>
       </c>
@@ -12349,7 +12349,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>214325</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>214376</v>
       </c>
@@ -12497,7 +12497,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>214382</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>214207</v>
       </c>
@@ -12645,7 +12645,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>214254</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>214341</v>
       </c>
@@ -12793,7 +12793,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>214391</v>
       </c>
@@ -12867,7 +12867,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>214241</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>214284</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>214309</v>
       </c>
@@ -13089,7 +13089,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>214316</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>214329</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>214332</v>
       </c>
@@ -13311,7 +13311,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>214338</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>214389</v>
       </c>
@@ -13459,7 +13459,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>214411</v>
       </c>
@@ -13533,7 +13533,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>214205</v>
       </c>
@@ -13607,7 +13607,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>214213</v>
       </c>
@@ -13681,7 +13681,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>214233</v>
       </c>
@@ -13755,7 +13755,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>214328</v>
       </c>
@@ -13829,7 +13829,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>214394</v>
       </c>
@@ -13903,7 +13903,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>214403</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>214410</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>214268</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>214438</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>214203</v>
       </c>
@@ -14273,7 +14273,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>214210</v>
       </c>
@@ -14347,7 +14347,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>214275</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>214304</v>
       </c>
@@ -14495,7 +14495,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>214337</v>
       </c>
@@ -14569,7 +14569,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>214202</v>
       </c>
@@ -14643,7 +14643,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>214212</v>
       </c>
@@ -14717,7 +14717,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>214219</v>
       </c>
@@ -14791,7 +14791,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>214288</v>
       </c>
@@ -14865,7 +14865,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>214315</v>
       </c>
@@ -14939,7 +14939,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>214318</v>
       </c>
@@ -15013,7 +15013,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>214327</v>
       </c>
@@ -15087,7 +15087,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>214336</v>
       </c>
@@ -15155,7 +15155,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>214385</v>
       </c>
@@ -15229,7 +15229,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>214442</v>
       </c>
@@ -15303,7 +15303,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>214330</v>
       </c>
@@ -15377,7 +15377,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>214366</v>
       </c>
@@ -15451,7 +15451,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>214368</v>
       </c>
@@ -15525,7 +15525,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>214375</v>
       </c>
@@ -15599,7 +15599,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>214381</v>
       </c>
@@ -15673,7 +15673,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>214390</v>
       </c>
@@ -15747,7 +15747,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>214395</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>214416</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>214200</v>
       </c>
@@ -15969,7 +15969,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>214294</v>
       </c>
@@ -16043,7 +16043,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>214347</v>
       </c>
@@ -16117,7 +16117,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>214407</v>
       </c>
@@ -16191,7 +16191,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>78487</v>
       </c>
@@ -16265,7 +16265,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>78488</v>
       </c>
@@ -16339,7 +16339,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>78501</v>
       </c>
@@ -16413,7 +16413,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>78499</v>
       </c>
@@ -16487,7 +16487,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>78476</v>
       </c>
@@ -16561,7 +16561,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>78489</v>
       </c>
@@ -16635,7 +16635,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>78480</v>
       </c>
@@ -16709,7 +16709,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>78497</v>
       </c>
@@ -16783,7 +16783,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>78498</v>
       </c>
@@ -16857,7 +16857,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>78490</v>
       </c>
@@ -16931,7 +16931,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>78502</v>
       </c>
@@ -17005,7 +17005,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>78504</v>
       </c>
@@ -17079,7 +17079,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>78481</v>
       </c>
@@ -17153,7 +17153,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>78508</v>
       </c>
@@ -17227,7 +17227,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>78511</v>
       </c>
@@ -17301,7 +17301,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>78494</v>
       </c>
@@ -17375,7 +17375,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>78486</v>
       </c>
@@ -17449,7 +17449,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>78491</v>
       </c>
@@ -17523,7 +17523,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>78507</v>
       </c>
@@ -17597,7 +17597,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>78482</v>
       </c>
@@ -17671,7 +17671,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>78483</v>
       </c>
@@ -17745,7 +17745,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>78503</v>
       </c>
@@ -17819,7 +17819,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>78479</v>
       </c>
@@ -17893,7 +17893,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>78477</v>
       </c>
@@ -17967,7 +17967,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>78510</v>
       </c>
@@ -18041,7 +18041,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>78506</v>
       </c>
@@ -18115,7 +18115,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>78484</v>
       </c>
@@ -18189,7 +18189,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>78492</v>
       </c>
@@ -18263,7 +18263,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>78505</v>
       </c>
@@ -18337,7 +18337,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>78500</v>
       </c>
@@ -18411,7 +18411,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>78475</v>
       </c>
@@ -18485,7 +18485,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>78485</v>
       </c>
@@ -18559,7 +18559,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>78512</v>
       </c>
@@ -18633,7 +18633,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>78493</v>
       </c>
@@ -18707,7 +18707,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>78509</v>
       </c>
@@ -18781,7 +18781,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>78495</v>
       </c>
@@ -18855,7 +18855,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>78496</v>
       </c>
@@ -18929,7 +18929,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>78478</v>
       </c>
@@ -19003,7 +19003,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>124467</v>
       </c>
@@ -19077,7 +19077,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>124473</v>
       </c>
@@ -19151,7 +19151,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>124469</v>
       </c>
@@ -19225,7 +19225,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>124463</v>
       </c>
@@ -19299,7 +19299,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>124475</v>
       </c>
@@ -19373,7 +19373,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>124464</v>
       </c>
@@ -19447,7 +19447,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>124476</v>
       </c>
@@ -19521,7 +19521,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>124468</v>
       </c>
@@ -19595,7 +19595,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>124472</v>
       </c>
@@ -19669,7 +19669,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>124466</v>
       </c>
@@ -19743,7 +19743,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>124471</v>
       </c>
@@ -19817,7 +19817,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>124477</v>
       </c>
@@ -19891,7 +19891,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>124465</v>
       </c>
@@ -19965,7 +19965,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>124470</v>
       </c>
@@ -20039,7 +20039,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>124474</v>
       </c>
@@ -20113,7 +20113,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>209133</v>
       </c>
@@ -20187,7 +20187,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>209143</v>
       </c>
@@ -20261,7 +20261,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>209132</v>
       </c>
@@ -20335,7 +20335,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>209136</v>
       </c>
@@ -20409,7 +20409,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>209137</v>
       </c>
@@ -20483,7 +20483,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>209141</v>
       </c>
@@ -20557,7 +20557,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>209142</v>
       </c>
@@ -20631,7 +20631,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>209145</v>
       </c>
@@ -20705,7 +20705,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>209138</v>
       </c>
@@ -20779,7 +20779,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>209140</v>
       </c>
@@ -20853,7 +20853,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>209135</v>
       </c>
@@ -20927,7 +20927,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>209134</v>
       </c>
@@ -21001,7 +21001,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>209144</v>
       </c>
@@ -21075,7 +21075,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>209139</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>209146</v>
       </c>
@@ -21223,7 +21223,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>211788</v>
       </c>
@@ -21297,7 +21297,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>211790</v>
       </c>
@@ -21371,7 +21371,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>211786</v>
       </c>
@@ -21445,7 +21445,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>211776</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>211773</v>
       </c>
@@ -21593,7 +21593,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>211784</v>
       </c>
@@ -21667,7 +21667,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>211789</v>
       </c>
@@ -21741,7 +21741,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>211781</v>
       </c>
@@ -21815,7 +21815,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>211780</v>
       </c>
@@ -21889,7 +21889,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>211787</v>
       </c>
@@ -21963,7 +21963,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>211778</v>
       </c>
@@ -22037,7 +22037,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>211785</v>
       </c>
@@ -22111,7 +22111,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>211775</v>
       </c>
@@ -22185,7 +22185,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>211772</v>
       </c>
@@ -22259,7 +22259,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>211774</v>
       </c>
@@ -22333,7 +22333,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>211779</v>
       </c>
@@ -22407,7 +22407,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>211777</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>211782</v>
       </c>
@@ -22555,7 +22555,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>211783</v>
       </c>
@@ -22629,7 +22629,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>16782</v>
       </c>
@@ -22703,7 +22703,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>16795</v>
       </c>
@@ -22787,12 +22787,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22981,15 +22978,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241AC70E-D880-4800-9004-A9D9AE6889BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA52FC2F-C454-413C-ABB0-35CDE4853AE6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d6067603-0566-4aef-af39-456c707b8d37"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b0fb223e-eed9-4298-9bf0-6173f7ec1518"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -23014,18 +23023,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA52FC2F-C454-413C-ABB0-35CDE4853AE6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241AC70E-D880-4800-9004-A9D9AE6889BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d6067603-0566-4aef-af39-456c707b8d37"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b0fb223e-eed9-4298-9bf0-6173f7ec1518"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>